<commit_message>
Added closure data to Excel file
</commit_message>
<xml_diff>
--- a/startup_analysis_post1990.xlsx
+++ b/startup_analysis_post1990.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Avg_founding_funding" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,19 @@
     <sheet name="Country_count" sheetId="4" r:id="rId4"/>
     <sheet name="Num_founded_per_year" sheetId="5" r:id="rId5"/>
     <sheet name="Companies_per_category" sheetId="6" r:id="rId6"/>
+    <sheet name="Avg_closure_country" sheetId="7" r:id="rId7"/>
+    <sheet name="Category_closure" sheetId="8" r:id="rId8"/>
+    <sheet name="Country_count_closure" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Avg_closure_country!$A$1:$B$148</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Avg_founding_funding!$A$1:$B$214</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Avg_funding_cat!$A$1:$B$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Avg_funding_country!$A$1:$D$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Category_closure!$A$1:$B$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Companies_per_category!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Country_count!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Country_count_closure!$A$1:$B$148</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Num_founded_per_year!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="353">
   <si>
     <t>Year</t>
   </si>
@@ -1079,18 +1085,38 @@
   </si>
   <si>
     <t>Nepal</t>
+  </si>
+  <si>
+    <t>Average Closure</t>
+  </si>
+  <si>
+    <t>Percentage Closed</t>
+  </si>
+  <si>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>Total Closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1146,33 +1172,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="18">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1190,6 +1218,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="17" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -6653,7 +6682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -7052,4 +7081,2940 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:B148"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" hidden="1">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" hidden="1">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" hidden="1">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" hidden="1">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" hidden="1">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" hidden="1">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" hidden="1">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" hidden="1">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1">
+      <c r="A10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" hidden="1">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" hidden="1">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" hidden="1">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" hidden="1">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" hidden="1">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" hidden="1">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1">
+      <c r="A17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" hidden="1">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1">
+      <c r="A24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1">
+      <c r="A25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" hidden="1">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" hidden="1">
+      <c r="A29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" hidden="1">
+      <c r="A30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1">
+      <c r="A32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" hidden="1">
+      <c r="A33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" hidden="1">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" hidden="1">
+      <c r="A35" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" hidden="1">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" hidden="1">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" hidden="1">
+      <c r="A38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" hidden="1">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" hidden="1">
+      <c r="A40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" hidden="1">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" hidden="1">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" hidden="1">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" hidden="1">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" hidden="1">
+      <c r="A45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" hidden="1">
+      <c r="A46" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" hidden="1">
+      <c r="A47" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" hidden="1">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" hidden="1">
+      <c r="A49" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" hidden="1">
+      <c r="A50" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" hidden="1">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" hidden="1">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" hidden="1">
+      <c r="A53" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" hidden="1">
+      <c r="A54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" hidden="1">
+      <c r="A55" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" hidden="1">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" hidden="1">
+      <c r="A57" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" hidden="1">
+      <c r="A58" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" hidden="1">
+      <c r="A59" t="s">
+        <v>158</v>
+      </c>
+      <c r="B59" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" hidden="1">
+      <c r="A60" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" hidden="1">
+      <c r="A61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" hidden="1">
+      <c r="A62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B62" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" hidden="1">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" hidden="1">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" hidden="1">
+      <c r="A65" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" hidden="1">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" hidden="1">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" hidden="1">
+      <c r="A68" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" hidden="1">
+      <c r="A69" t="s">
+        <v>51</v>
+      </c>
+      <c r="B69" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" hidden="1">
+      <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" hidden="1">
+      <c r="A71" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1">
+      <c r="A72" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" hidden="1">
+      <c r="A73" t="s">
+        <v>162</v>
+      </c>
+      <c r="B73" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" hidden="1">
+      <c r="A74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>110</v>
+      </c>
+      <c r="B75" s="5">
+        <v>2.6315789473684199E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="5">
+        <v>2.77777777777777E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" s="5">
+        <v>2.8864059590316501E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="5">
+        <v>2.94117647058823E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>60</v>
+      </c>
+      <c r="B79" s="5">
+        <v>2.94117647058823E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" s="5">
+        <v>3.06122448979591E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>115</v>
+      </c>
+      <c r="B81" s="5">
+        <v>3.2786885245901599E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>176</v>
+      </c>
+      <c r="B82" s="5">
+        <v>3.3333333333333298E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="5">
+        <v>3.5413153456998303E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>120</v>
+      </c>
+      <c r="B84" s="5">
+        <v>3.6332179930795801E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>59</v>
+      </c>
+      <c r="B85" s="5">
+        <v>3.72807017543859E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>148</v>
+      </c>
+      <c r="B86" s="5">
+        <v>3.7593984962405999E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>103</v>
+      </c>
+      <c r="B87" s="5">
+        <v>3.7735849056603703E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>145</v>
+      </c>
+      <c r="B88" s="5">
+        <v>3.9215686274509803E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>136</v>
+      </c>
+      <c r="B89" s="5">
+        <v>4.0740740740740702E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>58</v>
+      </c>
+      <c r="B90" s="5">
+        <v>4.1095890410958902E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>135</v>
+      </c>
+      <c r="B91" s="5">
+        <v>4.1237113402061799E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92" s="5">
+        <v>4.1322314049586702E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>187</v>
+      </c>
+      <c r="B93" s="5">
+        <v>4.1666666666666602E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>84</v>
+      </c>
+      <c r="B94" s="5">
+        <v>4.1832669322709098E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" s="5">
+        <v>4.2553191489361701E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>169</v>
+      </c>
+      <c r="B96" s="5">
+        <v>4.2857142857142802E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>181</v>
+      </c>
+      <c r="B97" s="5">
+        <v>4.3143297380585498E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>88</v>
+      </c>
+      <c r="B98" s="5">
+        <v>4.3478260869565202E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99" s="5">
+        <v>4.4117647058823498E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>77</v>
+      </c>
+      <c r="B100" s="5">
+        <v>4.5112781954887202E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" s="5">
+        <v>4.54545454545454E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>52</v>
+      </c>
+      <c r="B102" s="5">
+        <v>4.7138047138047097E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" s="5">
+        <v>4.71698113207547E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>151</v>
+      </c>
+      <c r="B104" s="5">
+        <v>4.7244094488188899E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>95</v>
+      </c>
+      <c r="B105" s="5">
+        <v>4.7619047619047603E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>150</v>
+      </c>
+      <c r="B106" s="5">
+        <v>5.0149253731343199E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>132</v>
+      </c>
+      <c r="B107" s="5">
+        <v>5.1094890510948898E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>63</v>
+      </c>
+      <c r="B108" s="5">
+        <v>5.1282051282051197E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>92</v>
+      </c>
+      <c r="B109" s="5">
+        <v>5.2469135802469098E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" s="5">
+        <v>5.2631578947368397E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>186</v>
+      </c>
+      <c r="B111" s="5">
+        <v>5.3333333333333302E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>124</v>
+      </c>
+      <c r="B112" s="5">
+        <v>5.4214123006833703E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>140</v>
+      </c>
+      <c r="B113" s="5">
+        <v>5.46875E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>74</v>
+      </c>
+      <c r="B114" s="5">
+        <v>5.4852320675105398E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>118</v>
+      </c>
+      <c r="B115" s="5">
+        <v>5.5555555555555497E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>166</v>
+      </c>
+      <c r="B116" s="5">
+        <v>5.5555555555555497E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>179</v>
+      </c>
+      <c r="B117" s="5">
+        <v>5.5555555555555497E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>183</v>
+      </c>
+      <c r="B118" s="5">
+        <v>5.61569688768606E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>153</v>
+      </c>
+      <c r="B119" s="5">
+        <v>5.7324840764331197E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>55</v>
+      </c>
+      <c r="B120" s="5">
+        <v>5.8823529411764698E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>116</v>
+      </c>
+      <c r="B121" s="5">
+        <v>5.8823529411764698E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>114</v>
+      </c>
+      <c r="B122" s="5">
+        <v>5.9791332263242299E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>91</v>
+      </c>
+      <c r="B123" s="5">
+        <v>6.0606060606060601E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>53</v>
+      </c>
+      <c r="B124" s="5">
+        <v>6.1769616026711098E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>165</v>
+      </c>
+      <c r="B125" s="5">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>105</v>
+      </c>
+      <c r="B126" s="5">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>161</v>
+      </c>
+      <c r="B127" s="5">
+        <v>6.4516129032257993E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>76</v>
+      </c>
+      <c r="B128" s="5">
+        <v>6.5420560747663503E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>141</v>
+      </c>
+      <c r="B129" s="5">
+        <v>6.6666666666666596E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>121</v>
+      </c>
+      <c r="B130" s="5">
+        <v>6.7415730337078594E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" s="5">
+        <v>6.7437379576107903E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>147</v>
+      </c>
+      <c r="B132" s="5">
+        <v>6.7796610169491497E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>117</v>
+      </c>
+      <c r="B133" s="5">
+        <v>7.1428571428571397E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>127</v>
+      </c>
+      <c r="B134" s="5">
+        <v>7.1428571428571397E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>142</v>
+      </c>
+      <c r="B135" s="5">
+        <v>7.15667311411992E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>68</v>
+      </c>
+      <c r="B136" s="5">
+        <v>7.3170731707316999E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>144</v>
+      </c>
+      <c r="B137" s="5">
+        <v>7.4667001759235893E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" s="5">
+        <v>7.69230769230769E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>73</v>
+      </c>
+      <c r="B139" s="5">
+        <v>7.69230769230769E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>163</v>
+      </c>
+      <c r="B140" s="5">
+        <v>8.3333333333333301E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>191</v>
+      </c>
+      <c r="B141" s="5">
+        <v>9.0909090909090898E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>78</v>
+      </c>
+      <c r="B142" s="5">
+        <v>9.2592592592592504E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>75</v>
+      </c>
+      <c r="B143" s="5">
+        <v>9.38967136150234E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>184</v>
+      </c>
+      <c r="B144" s="5">
+        <v>0.106741573033707</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>195</v>
+      </c>
+      <c r="B145" s="5">
+        <v>0.16666666666666599</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>107</v>
+      </c>
+      <c r="B146" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>177</v>
+      </c>
+      <c r="B147" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>126</v>
+      </c>
+      <c r="B148" s="5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B148">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="10.674%"/>
+        <filter val="100.000%"/>
+        <filter val="16.667%"/>
+        <filter val="2.632%"/>
+        <filter val="2.778%"/>
+        <filter val="2.886%"/>
+        <filter val="2.941%"/>
+        <filter val="3.061%"/>
+        <filter val="3.279%"/>
+        <filter val="3.333%"/>
+        <filter val="3.541%"/>
+        <filter val="3.633%"/>
+        <filter val="3.728%"/>
+        <filter val="3.759%"/>
+        <filter val="3.774%"/>
+        <filter val="3.922%"/>
+        <filter val="4.074%"/>
+        <filter val="4.110%"/>
+        <filter val="4.124%"/>
+        <filter val="4.132%"/>
+        <filter val="4.167%"/>
+        <filter val="4.183%"/>
+        <filter val="4.255%"/>
+        <filter val="4.286%"/>
+        <filter val="4.314%"/>
+        <filter val="4.348%"/>
+        <filter val="4.412%"/>
+        <filter val="4.511%"/>
+        <filter val="4.545%"/>
+        <filter val="4.714%"/>
+        <filter val="4.717%"/>
+        <filter val="4.724%"/>
+        <filter val="4.762%"/>
+        <filter val="5.015%"/>
+        <filter val="5.109%"/>
+        <filter val="5.128%"/>
+        <filter val="5.247%"/>
+        <filter val="5.263%"/>
+        <filter val="5.333%"/>
+        <filter val="5.421%"/>
+        <filter val="5.469%"/>
+        <filter val="5.485%"/>
+        <filter val="5.556%"/>
+        <filter val="5.616%"/>
+        <filter val="5.732%"/>
+        <filter val="5.882%"/>
+        <filter val="5.979%"/>
+        <filter val="50.000%"/>
+        <filter val="6.061%"/>
+        <filter val="6.177%"/>
+        <filter val="6.250%"/>
+        <filter val="6.452%"/>
+        <filter val="6.542%"/>
+        <filter val="6.667%"/>
+        <filter val="6.742%"/>
+        <filter val="6.744%"/>
+        <filter val="6.780%"/>
+        <filter val="7.143%"/>
+        <filter val="7.157%"/>
+        <filter val="7.317%"/>
+        <filter val="7.467%"/>
+        <filter val="7.692%"/>
+        <filter val="8.333%"/>
+        <filter val="9.091%"/>
+        <filter val="9.259%"/>
+        <filter val="9.390%"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:B148">
+      <sortCondition ref="B1:B148"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2.0454545454545399E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2.5391680172879499E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3.5876993166287001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3.6431574030826697E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4.2747021723896203E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5">
+        <v>4.3970944309927297E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4.4556234279554401E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5">
+        <v>4.8988285410010601E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5.02803738317757E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5.0314465408804999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5">
+        <v>5.0671654480530501E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="5">
+        <v>5.1418225709112801E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5.3503184713375798E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5">
+        <v>5.36423841059602E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="5">
+        <v>5.5201021059349001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="5">
+        <v>5.5347793567688798E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="5">
+        <v>5.5772448410485197E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5.7086614173228301E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5.8823529411764698E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="5">
+        <v>5.8984760442933798E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="5">
+        <v>5.9749884205650701E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="5">
+        <v>6.0039370078740099E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5">
+        <v>6.00877192982456E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5">
+        <v>6.1554695743932401E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="5">
+        <v>6.3051439986682195E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="5">
+        <v>6.5959409594095894E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="5">
+        <v>6.7060810810810806E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="5">
+        <v>6.8017863277224297E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="5">
+        <v>6.8563482725425104E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="5">
+        <v>6.9746376811594193E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="5">
+        <v>7.0337521557033697E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="5">
+        <v>7.1020408163265297E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="5">
+        <v>7.3902516054321493E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="5">
+        <v>7.4360960495739703E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="5">
+        <v>7.9703130041948997E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="5">
+        <v>8.2474226804123696E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="5">
+        <v>8.2905982905982903E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5">
+        <v>8.7382605144957104E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="5">
+        <v>8.9480048367593698E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="5">
+        <v>9.1145833333333301E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="5">
+        <v>9.1614612909331802E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="5">
+        <v>9.6045197740112997E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="5">
+        <v>9.7293814432989595E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0.10179153094462499</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B47">
+    <sortState ref="A2:B47">
+      <sortCondition ref="B1:B47"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:B148"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" hidden="1">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" hidden="1">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" hidden="1">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" hidden="1">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" hidden="1">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" hidden="1">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" hidden="1">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" hidden="1">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1">
+      <c r="A10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" hidden="1">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" hidden="1">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" hidden="1">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" hidden="1">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" hidden="1">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" hidden="1">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1">
+      <c r="A17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" hidden="1">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1">
+      <c r="A24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1">
+      <c r="A25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" hidden="1">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" hidden="1">
+      <c r="A29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" hidden="1">
+      <c r="A30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1">
+      <c r="A32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" hidden="1">
+      <c r="A33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" hidden="1">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" hidden="1">
+      <c r="A35" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" hidden="1">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" hidden="1">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" hidden="1">
+      <c r="A38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" hidden="1">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" hidden="1">
+      <c r="A40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" hidden="1">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" hidden="1">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" hidden="1">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" hidden="1">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" hidden="1">
+      <c r="A45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" hidden="1">
+      <c r="A46" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" hidden="1">
+      <c r="A47" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" hidden="1">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" hidden="1">
+      <c r="A49" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" hidden="1">
+      <c r="A50" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" hidden="1">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" hidden="1">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" hidden="1">
+      <c r="A53" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" hidden="1">
+      <c r="A54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" hidden="1">
+      <c r="A55" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" hidden="1">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" hidden="1">
+      <c r="A57" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" hidden="1">
+      <c r="A58" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" hidden="1">
+      <c r="A59" t="s">
+        <v>158</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" hidden="1">
+      <c r="A60" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" hidden="1">
+      <c r="A61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" hidden="1">
+      <c r="A62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" hidden="1">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" hidden="1">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" hidden="1">
+      <c r="A65" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" hidden="1">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" hidden="1">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" hidden="1">
+      <c r="A68" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" hidden="1">
+      <c r="A69" t="s">
+        <v>51</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" hidden="1">
+      <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" hidden="1">
+      <c r="A71" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1">
+      <c r="A72" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" hidden="1">
+      <c r="A73" t="s">
+        <v>162</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" hidden="1">
+      <c r="A74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>163</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>110</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>195</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>141</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>179</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>126</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>73</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>177</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>116</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>127</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>115</v>
+      </c>
+      <c r="B93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>125</v>
+      </c>
+      <c r="B94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>139</v>
+      </c>
+      <c r="B95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>58</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>105</v>
+      </c>
+      <c r="B99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>161</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>100</v>
+      </c>
+      <c r="B103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>186</v>
+      </c>
+      <c r="B104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>147</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>103</v>
+      </c>
+      <c r="B106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>97</v>
+      </c>
+      <c r="B107">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>78</v>
+      </c>
+      <c r="B108">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>148</v>
+      </c>
+      <c r="B109">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>63</v>
+      </c>
+      <c r="B110">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>68</v>
+      </c>
+      <c r="B111">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>145</v>
+      </c>
+      <c r="B112">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>151</v>
+      </c>
+      <c r="B114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>169</v>
+      </c>
+      <c r="B115">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>166</v>
+      </c>
+      <c r="B116">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>165</v>
+      </c>
+      <c r="B117">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>135</v>
+      </c>
+      <c r="B118">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>108</v>
+      </c>
+      <c r="B119">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>153</v>
+      </c>
+      <c r="B120">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>94</v>
+      </c>
+      <c r="B121">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>77</v>
+      </c>
+      <c r="B122">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>176</v>
+      </c>
+      <c r="B123">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>187</v>
+      </c>
+      <c r="B124">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>79</v>
+      </c>
+      <c r="B125">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>92</v>
+      </c>
+      <c r="B126">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>59</v>
+      </c>
+      <c r="B127">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>184</v>
+      </c>
+      <c r="B128">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>75</v>
+      </c>
+      <c r="B129">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>120</v>
+      </c>
+      <c r="B130">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>76</v>
+      </c>
+      <c r="B131">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>130</v>
+      </c>
+      <c r="B133">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>84</v>
+      </c>
+      <c r="B134">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>140</v>
+      </c>
+      <c r="B135">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>181</v>
+      </c>
+      <c r="B136">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>168</v>
+      </c>
+      <c r="B138">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>142</v>
+      </c>
+      <c r="B139">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>52</v>
+      </c>
+      <c r="B140">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>119</v>
+      </c>
+      <c r="B141">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>74</v>
+      </c>
+      <c r="B142">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>53</v>
+      </c>
+      <c r="B143">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>183</v>
+      </c>
+      <c r="B144">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>150</v>
+      </c>
+      <c r="B145">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>124</v>
+      </c>
+      <c r="B146">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>114</v>
+      </c>
+      <c r="B147">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>144</v>
+      </c>
+      <c r="B148">
+        <v>2971</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B148">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+        <filter val="10"/>
+        <filter val="119"/>
+        <filter val="12"/>
+        <filter val="14"/>
+        <filter val="15"/>
+        <filter val="17"/>
+        <filter val="19"/>
+        <filter val="2"/>
+        <filter val="20"/>
+        <filter val="21"/>
+        <filter val="28"/>
+        <filter val="2971"/>
+        <filter val="298"/>
+        <filter val="3"/>
+        <filter val="33"/>
+        <filter val="35"/>
+        <filter val="37"/>
+        <filter val="4"/>
+        <filter val="42"/>
+        <filter val="5"/>
+        <filter val="6"/>
+        <filter val="62"/>
+        <filter val="65"/>
+        <filter val="7"/>
+        <filter val="74"/>
+        <filter val="8"/>
+        <filter val="83"/>
+        <filter val="84"/>
+        <filter val="9"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:B148">
+      <sortCondition ref="B1:B148"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>